<commit_message>
Updated isolator part number.
</commit_message>
<xml_diff>
--- a/PCB/CAM_OUTPUTS/BOM/FLEXI_HAL_2000_CAM_OUTPUT_A4.xlsx
+++ b/PCB/CAM_OUTPUTS/BOM/FLEXI_HAL_2000_CAM_OUTPUT_A4.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repo\cnc_projects\STM32F446CE_CNC_BOARD\Project Outputs for FLEXI_HAL_2000\FLEXI_HAL_2000_UPLOAD_GERBERS_A4\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repo\Flexi-HAL\PCB\CAM_OUTPUTS\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -872,12 +872,6 @@
     <t>Dual Channel Isolator</t>
   </si>
   <si>
-    <t>C476471</t>
-  </si>
-  <si>
-    <t>CBMuD1200HAS8</t>
-  </si>
-  <si>
     <t>U9, U12, U13, U15, U16, U17, U29, U31, U33</t>
   </si>
   <si>
@@ -1027,6 +1021,12 @@
   <si>
     <t xml:space="preserve">
 C66690</t>
+  </si>
+  <si>
+    <t>C476470</t>
+  </si>
+  <si>
+    <t>CBMuD1200LAS8</t>
   </si>
 </sst>
 </file>
@@ -1374,8 +1374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2377,7 +2377,7 @@
         <v>184</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="2" t="s">
@@ -2993,16 +2993,16 @@
         <v>280</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>281</v>
+        <v>331</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>279</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>282</v>
+        <v>332</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="I62" s="2" t="s">
         <v>279</v>
@@ -3015,22 +3015,22 @@
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="F63" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="E63" s="2" t="s">
+      <c r="G63" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="F63" s="2" t="s">
+      <c r="H63" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="G63" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="H63" s="2" t="s">
-        <v>288</v>
-      </c>
       <c r="I63" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -3040,19 +3040,19 @@
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>279</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="I64" s="2" t="s">
         <v>279</v>
@@ -3063,28 +3063,28 @@
         <v>3</v>
       </c>
       <c r="B65" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="D65" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="E65" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="D65" s="2" t="s">
+      <c r="F65" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="G65" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="E65" s="2" t="s">
+      <c r="H65" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="F65" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="G65" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="H65" s="2" t="s">
-        <v>298</v>
-      </c>
       <c r="I65" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -3092,28 +3092,28 @@
         <v>1</v>
       </c>
       <c r="B66" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D66" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="E66" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="D66" s="2" t="s">
+      <c r="F66" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="E66" s="2" t="s">
+      <c r="G66" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="H66" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="F66" s="2" t="s">
+      <c r="I66" s="2" t="s">
         <v>303</v>
-      </c>
-      <c r="G66" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="H66" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="I66" s="2" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -3123,19 +3123,19 @@
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>279</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="I67" s="2" t="s">
         <v>279</v>
@@ -3148,20 +3148,20 @@
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F68" s="1"/>
       <c r="G68" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="I68" s="2" t="s">
         <v>312</v>
-      </c>
-      <c r="H68" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="I68" s="2" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -3171,22 +3171,22 @@
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="F69" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="E69" s="2" t="s">
+      <c r="G69" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="F69" s="2" t="s">
+      <c r="H69" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="G69" s="2" t="s">
+      <c r="I69" s="2" t="s">
         <v>318</v>
-      </c>
-      <c r="H69" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="I69" s="2" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -3194,28 +3194,28 @@
         <v>1</v>
       </c>
       <c r="B70" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="D70" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="E70" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="D70" s="2" t="s">
+      <c r="F70" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="E70" s="2" t="s">
+      <c r="G70" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="H70" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="F70" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="G70" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="H70" s="2" t="s">
-        <v>326</v>
-      </c>
       <c r="I70" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -3225,20 +3225,20 @@
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="F71" s="1"/>
       <c r="G71" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="H71" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="I71" s="2" t="s">
         <v>329</v>
-      </c>
-      <c r="H71" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="I71" s="2" t="s">
-        <v>331</v>
       </c>
     </row>
   </sheetData>

</xml_diff>